<commit_message>
them vai thu để viet report
</commit_message>
<xml_diff>
--- a/Genentic_Analysis/Result.xlsx
+++ b/Genentic_Analysis/Result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test</t>
   </si>
@@ -24,18 +24,15 @@
   <si>
     <t>Method 2</t>
   </si>
-  <si>
-    <t>Method 3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -55,46 +52,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,14 +68,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,6 +107,36 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -138,13 +151,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -153,9 +159,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,23 +175,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,8 +188,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,187 +205,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,6 +396,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,17 +447,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,24 +488,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -475,42 +496,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -523,127 +520,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -761,10 +758,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$22</c:f>
+              <c:f>Sheet1!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>723</c:v>
                 </c:pt>
@@ -775,57 +772,60 @@
                   <c:v>2230</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2811</c:v>
+                  <c:v>3086</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4232</c:v>
+                  <c:v>4771</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3857</c:v>
+                  <c:v>4480</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6185</c:v>
+                  <c:v>7316</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6616</c:v>
+                  <c:v>8206</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4469</c:v>
+                  <c:v>6022</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5724</c:v>
+                  <c:v>7096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17137</c:v>
+                  <c:v>20921</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29005</c:v>
+                  <c:v>33369</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46663</c:v>
+                  <c:v>50751</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55822</c:v>
+                  <c:v>61359</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>75578</c:v>
+                  <c:v>77012</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83056</c:v>
+                  <c:v>92976</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>99780</c:v>
+                  <c:v>104262</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>114221</c:v>
+                  <c:v>121673</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>121987</c:v>
+                  <c:v>131679</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>140843</c:v>
+                  <c:v>146765</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
@@ -861,10 +861,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$22</c:f>
+              <c:f>Sheet1!$C$2:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>723</c:v>
                 </c:pt>
@@ -872,160 +872,63 @@
                   <c:v>2414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2120</c:v>
+                  <c:v>2181</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2980</c:v>
+                  <c:v>3083</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4187</c:v>
+                  <c:v>4705</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3903</c:v>
+                  <c:v>4619</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6417</c:v>
+                  <c:v>7143</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6777</c:v>
+                  <c:v>8009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4739</c:v>
+                  <c:v>6036</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5328</c:v>
+                  <c:v>6522</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16710</c:v>
+                  <c:v>21047</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30481</c:v>
+                  <c:v>35961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46605</c:v>
+                  <c:v>52505</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60671</c:v>
+                  <c:v>64305</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>72842</c:v>
+                  <c:v>78211</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>82227</c:v>
+                  <c:v>89140</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>98526</c:v>
+                  <c:v>104570</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>112893</c:v>
+                  <c:v>124046</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>123912</c:v>
+                  <c:v>133593</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>141457</c:v>
+                  <c:v>148337</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>-1</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Method 3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>723</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2414</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2071</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3055</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3920</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6670</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6912</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4853</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5581</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16922</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29208</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>46280</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>56891</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>73273</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>84057</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>96376</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>111687</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>126825</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>140310</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2060,10 +1963,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -2082,11 +1985,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2096,11 +1997,8 @@
       <c r="C2">
         <v>723</v>
       </c>
-      <c r="D2">
-        <v>723</v>
-      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2110,11 +2008,8 @@
       <c r="C3">
         <v>2414</v>
       </c>
-      <c r="D3">
-        <v>2414</v>
-      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2122,251 +2017,197 @@
         <v>2230</v>
       </c>
       <c r="C4">
-        <v>2120</v>
-      </c>
-      <c r="D4">
-        <v>2071</v>
+        <v>2181</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2811</v>
+        <v>3086</v>
       </c>
       <c r="C5">
-        <v>2980</v>
-      </c>
-      <c r="D5">
-        <v>3055</v>
+        <v>3083</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4232</v>
+        <v>4771</v>
       </c>
       <c r="C6">
-        <v>4187</v>
-      </c>
-      <c r="D6">
-        <v>4200</v>
+        <v>4705</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3857</v>
+        <v>4480</v>
       </c>
       <c r="C7">
-        <v>3903</v>
-      </c>
-      <c r="D7">
-        <v>3920</v>
+        <v>4619</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6185</v>
+        <v>7316</v>
       </c>
       <c r="C8">
-        <v>6417</v>
-      </c>
-      <c r="D8">
-        <v>6670</v>
+        <v>7143</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6616</v>
+        <v>8206</v>
       </c>
       <c r="C9">
-        <v>6777</v>
-      </c>
-      <c r="D9">
-        <v>6912</v>
+        <v>8009</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4469</v>
+        <v>6022</v>
       </c>
       <c r="C10">
-        <v>4739</v>
-      </c>
-      <c r="D10">
-        <v>4853</v>
+        <v>6036</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5724</v>
+        <v>7096</v>
       </c>
       <c r="C11">
-        <v>5328</v>
-      </c>
-      <c r="D11">
-        <v>5581</v>
+        <v>6522</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>17137</v>
+        <v>20921</v>
       </c>
       <c r="C12">
-        <v>16710</v>
-      </c>
-      <c r="D12">
-        <v>16922</v>
+        <v>21047</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>29005</v>
+        <v>33369</v>
       </c>
       <c r="C13">
-        <v>30481</v>
-      </c>
-      <c r="D13">
-        <v>29208</v>
+        <v>35961</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>46663</v>
+        <v>50751</v>
       </c>
       <c r="C14">
-        <v>46605</v>
-      </c>
-      <c r="D14">
-        <v>46280</v>
+        <v>52505</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>55822</v>
+        <v>61359</v>
       </c>
       <c r="C15">
-        <v>60671</v>
-      </c>
-      <c r="D15">
-        <v>56891</v>
+        <v>64305</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>75578</v>
+        <v>77012</v>
       </c>
       <c r="C16">
-        <v>72842</v>
-      </c>
-      <c r="D16">
-        <v>73273</v>
+        <v>78211</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>83056</v>
+        <v>92976</v>
       </c>
       <c r="C17">
-        <v>82227</v>
-      </c>
-      <c r="D17">
-        <v>84057</v>
+        <v>89140</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>99780</v>
+        <v>104262</v>
       </c>
       <c r="C18">
-        <v>98526</v>
-      </c>
-      <c r="D18">
-        <v>96376</v>
+        <v>104570</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>114221</v>
+        <v>121673</v>
       </c>
       <c r="C19">
-        <v>112893</v>
-      </c>
-      <c r="D19">
-        <v>111687</v>
+        <v>124046</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>121987</v>
+        <v>131679</v>
       </c>
       <c r="C20">
-        <v>123912</v>
-      </c>
-      <c r="D20">
-        <v>126825</v>
+        <v>133593</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>140843</v>
+        <v>146765</v>
       </c>
       <c r="C21">
-        <v>141457</v>
-      </c>
-      <c r="D21">
-        <v>140310</v>
+        <v>148337</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2376,7 +2217,15 @@
       <c r="C22">
         <v>-1</v>
       </c>
-      <c r="D22">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>-1</v>
+      </c>
+      <c r="C23">
         <v>-1</v>
       </c>
     </row>

</xml_diff>